<commit_message>
petita modificació a experiments de k i numbins
</commit_message>
<xml_diff>
--- a/coses per l'informe/train test.xlsx
+++ b/coses per l'informe/train test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuari\Desktop\Documents\UNI\Q8\VC\projecte\ProjecteVC\coses per l'informe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E29EFA-C653-491E-B32E-61DC3DCF2177}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7025338F-ED32-4A62-997F-D5586B1B67E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{29E68929-73A9-4979-9760-6C8E267CED5D}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Madrid</t>
   </si>
   <si>
-    <t>TRAIN</t>
-  </si>
-  <si>
     <t>TEST</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>VALIDACIÓ</t>
+  </si>
+  <si>
+    <t>ENTRENAMENT</t>
   </si>
 </sst>
 </file>
@@ -185,17 +185,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2262B8-4C6F-4228-94C6-75734BA19B54}">
-  <dimension ref="E3:AM19"/>
+  <dimension ref="E3:AM17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="AI20" sqref="AI20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,53 +527,53 @@
   </cols>
   <sheetData>
     <row r="3" spans="5:39" x14ac:dyDescent="0.25">
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="5:39" x14ac:dyDescent="0.25">
+      <c r="E4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" spans="5:39" x14ac:dyDescent="0.25">
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="10"/>
-      <c r="AB4" s="10"/>
-      <c r="AC4" s="10"/>
-      <c r="AD4" s="10"/>
-      <c r="AE4" s="10"/>
-      <c r="AF4" s="10"/>
-      <c r="AG4" s="10"/>
-      <c r="AH4" s="10"/>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="10"/>
-      <c r="AK4" s="10"/>
-      <c r="AL4" s="10"/>
-      <c r="AM4" s="10"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="15"/>
+      <c r="AB4" s="15"/>
+      <c r="AC4" s="15"/>
+      <c r="AD4" s="15"/>
+      <c r="AE4" s="15"/>
+      <c r="AF4" s="15"/>
+      <c r="AG4" s="15"/>
+      <c r="AH4" s="15"/>
+      <c r="AI4" s="15"/>
+      <c r="AJ4" s="15"/>
+      <c r="AK4" s="15"/>
+      <c r="AL4" s="15"/>
+      <c r="AM4" s="15"/>
     </row>
     <row r="5" spans="5:39" x14ac:dyDescent="0.25">
       <c r="E5" s="7"/>
@@ -603,312 +603,309 @@
         <v>5</v>
       </c>
       <c r="AJ6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="5:39" x14ac:dyDescent="0.25">
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="11"/>
+      <c r="G7" s="9"/>
       <c r="H7" s="3"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
-      <c r="Z7" s="13"/>
-      <c r="AA7" s="13"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
-      <c r="AE7" s="13"/>
-      <c r="AF7" s="13"/>
+      <c r="AE7" s="11"/>
+      <c r="AF7" s="11"/>
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
-      <c r="AJ7" s="13"/>
-      <c r="AK7" s="13"/>
+      <c r="AJ7" s="11"/>
+      <c r="AK7" s="11"/>
       <c r="AL7" s="2"/>
       <c r="AM7" s="2"/>
     </row>
     <row r="8" spans="5:39" x14ac:dyDescent="0.25">
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="11"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="3"/>
       <c r="J8" s="8"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
-      <c r="Z8" s="13"/>
-      <c r="AA8" s="13"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
-      <c r="AE8" s="13"/>
-      <c r="AF8" s="13"/>
+      <c r="AE8" s="11"/>
+      <c r="AF8" s="11"/>
       <c r="AG8" s="2"/>
       <c r="AH8" s="2"/>
-      <c r="AJ8" s="13"/>
-      <c r="AK8" s="13"/>
+      <c r="AJ8" s="11"/>
+      <c r="AK8" s="11"/>
       <c r="AL8" s="2"/>
       <c r="AM8" s="2"/>
     </row>
     <row r="9" spans="5:39" x14ac:dyDescent="0.25">
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="11"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="3"/>
       <c r="J9" s="8"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
-      <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
-      <c r="Z9" s="13"/>
-      <c r="AA9" s="13"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="11"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
-      <c r="AE9" s="13"/>
-      <c r="AF9" s="13"/>
+      <c r="AE9" s="11"/>
+      <c r="AF9" s="11"/>
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
-      <c r="AJ9" s="13"/>
-      <c r="AK9" s="13"/>
+      <c r="AJ9" s="11"/>
+      <c r="AK9" s="11"/>
       <c r="AL9" s="2"/>
       <c r="AM9" s="2"/>
     </row>
     <row r="10" spans="5:39" x14ac:dyDescent="0.25">
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="11"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="3"/>
       <c r="J10" s="8"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
-      <c r="Z10" s="13"/>
-      <c r="AA10" s="13"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
-      <c r="AE10" s="13"/>
-      <c r="AF10" s="13"/>
+      <c r="AE10" s="11"/>
+      <c r="AF10" s="11"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
-      <c r="AJ10" s="13"/>
-      <c r="AK10" s="13"/>
+      <c r="AJ10" s="11"/>
+      <c r="AK10" s="11"/>
       <c r="AL10" s="2"/>
       <c r="AM10" s="2"/>
     </row>
     <row r="11" spans="5:39" x14ac:dyDescent="0.25">
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="11"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="3"/>
       <c r="J11" s="8"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="13"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
-      <c r="AE11" s="13"/>
-      <c r="AF11" s="13"/>
+      <c r="AE11" s="11"/>
+      <c r="AF11" s="11"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
-      <c r="AJ11" s="13"/>
-      <c r="AK11" s="13"/>
+      <c r="AJ11" s="11"/>
+      <c r="AK11" s="11"/>
       <c r="AL11" s="2"/>
       <c r="AM11" s="2"/>
     </row>
     <row r="12" spans="5:39" x14ac:dyDescent="0.25">
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="11"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="3"/>
       <c r="J12" s="8"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
-      <c r="U12" s="13"/>
-      <c r="V12" s="13"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
-      <c r="Z12" s="13"/>
-      <c r="AA12" s="13"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="11"/>
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
-      <c r="AE12" s="13"/>
-      <c r="AF12" s="13"/>
+      <c r="AE12" s="11"/>
+      <c r="AF12" s="11"/>
       <c r="AG12" s="2"/>
       <c r="AH12" s="2"/>
-      <c r="AJ12" s="13"/>
-      <c r="AK12" s="13"/>
+      <c r="AJ12" s="11"/>
+      <c r="AK12" s="11"/>
       <c r="AL12" s="2"/>
       <c r="AM12" s="2"/>
     </row>
     <row r="13" spans="5:39" x14ac:dyDescent="0.25">
       <c r="E13" s="1"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="11"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="3"/>
       <c r="J13" s="8"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
-      <c r="U13" s="13"/>
-      <c r="V13" s="13"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
-      <c r="Z13" s="13"/>
-      <c r="AA13" s="13"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="11"/>
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
-      <c r="AE13" s="13"/>
-      <c r="AF13" s="13"/>
+      <c r="AE13" s="11"/>
+      <c r="AF13" s="11"/>
       <c r="AG13" s="2"/>
       <c r="AH13" s="2"/>
-      <c r="AJ13" s="13"/>
-      <c r="AK13" s="13"/>
+      <c r="AJ13" s="11"/>
+      <c r="AK13" s="11"/>
       <c r="AL13" s="2"/>
       <c r="AM13" s="2"/>
     </row>
     <row r="14" spans="5:39" x14ac:dyDescent="0.25">
       <c r="E14" s="1"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="11"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="9"/>
       <c r="H14" s="3"/>
       <c r="J14" s="8"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
-      <c r="U14" s="13"/>
-      <c r="V14" s="13"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
-      <c r="Z14" s="13"/>
-      <c r="AA14" s="13"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
-      <c r="AE14" s="13"/>
-      <c r="AF14" s="13"/>
+      <c r="AE14" s="11"/>
+      <c r="AF14" s="11"/>
       <c r="AG14" s="2"/>
       <c r="AH14" s="2"/>
-      <c r="AJ14" s="13"/>
-      <c r="AK14" s="13"/>
+      <c r="AJ14" s="11"/>
+      <c r="AK14" s="11"/>
       <c r="AL14" s="2"/>
       <c r="AM14" s="2"/>
     </row>
     <row r="15" spans="5:39" x14ac:dyDescent="0.25">
       <c r="E15" s="1"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="11"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="3"/>
       <c r="J15" s="8"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
-      <c r="U15" s="13"/>
-      <c r="V15" s="13"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
-      <c r="Z15" s="13"/>
-      <c r="AA15" s="13"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
-      <c r="AE15" s="13"/>
-      <c r="AF15" s="13"/>
+      <c r="AE15" s="11"/>
+      <c r="AF15" s="11"/>
       <c r="AG15" s="2"/>
       <c r="AH15" s="2"/>
-      <c r="AJ15" s="13"/>
-      <c r="AK15" s="13"/>
+      <c r="AJ15" s="11"/>
+      <c r="AK15" s="11"/>
       <c r="AL15" s="2"/>
       <c r="AM15" s="2"/>
     </row>
     <row r="16" spans="5:39" x14ac:dyDescent="0.25">
-      <c r="J16" s="8"/>
-    </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E17" s="6" t="s">
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="27:39" x14ac:dyDescent="0.25">
+      <c r="AA17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="4"/>
+      <c r="AG17" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH17" s="13"/>
+      <c r="AI17" s="13"/>
+      <c r="AJ17" s="13"/>
+      <c r="AL17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-    </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E18" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-    </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E19" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="5"/>
+      <c r="AM17" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
experiment numbins hs hsv
</commit_message>
<xml_diff>
--- a/coses per l'informe/train test.xlsx
+++ b/coses per l'informe/train test.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuari\Desktop\Documents\UNI\Q8\VC\projecte\ProjecteVC\coses per l'informe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7025338F-ED32-4A62-997F-D5586B1B67E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428D2BBB-BDFA-4433-B661-928D8573316C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{29E68929-73A9-4979-9760-6C8E267CED5D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{29E68929-73A9-4979-9760-6C8E267CED5D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="entrega 1" sheetId="1" r:id="rId1"/>
+    <sheet name="entrega 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Barça</t>
   </si>
@@ -73,13 +74,34 @@
   </si>
   <si>
     <t>ENTRENAMENT</t>
+  </si>
+  <si>
+    <t>acmilan</t>
+  </si>
+  <si>
+    <t>barcelona</t>
+  </si>
+  <si>
+    <t>juventus</t>
+  </si>
+  <si>
+    <t>madrid</t>
+  </si>
+  <si>
+    <t>psv</t>
+  </si>
+  <si>
+    <t>chelsea</t>
+  </si>
+  <si>
+    <t>liverpool</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,8 +123,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +153,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF70AD47"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9BC2E6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -173,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -196,6 +237,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -204,6 +263,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9BC2E6"/>
+      <color rgb="FF70AD47"/>
       <color rgb="FFFF5757"/>
     </mruColors>
   </colors>
@@ -517,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2262B8-4C6F-4228-94C6-75734BA19B54}">
   <dimension ref="E3:AM17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI20" sqref="AI20"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,4 +977,580 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4754969A-F369-4511-A378-0DBA819E5C09}">
+  <dimension ref="D2:AX11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AE15" sqref="AE15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="3.140625" style="16"/>
+    <col min="5" max="50" width="2.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:50" x14ac:dyDescent="0.25">
+      <c r="E2" s="23">
+        <v>1</v>
+      </c>
+      <c r="F2" s="23">
+        <v>2</v>
+      </c>
+      <c r="G2" s="23">
+        <v>3</v>
+      </c>
+      <c r="H2" s="23">
+        <v>4</v>
+      </c>
+      <c r="I2" s="23">
+        <v>5</v>
+      </c>
+      <c r="J2" s="23">
+        <v>6</v>
+      </c>
+      <c r="K2" s="23">
+        <v>7</v>
+      </c>
+      <c r="L2" s="23">
+        <v>8</v>
+      </c>
+      <c r="M2" s="23">
+        <v>9</v>
+      </c>
+      <c r="N2" s="23">
+        <v>10</v>
+      </c>
+      <c r="O2" s="23">
+        <v>11</v>
+      </c>
+      <c r="P2" s="23">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="23">
+        <v>13</v>
+      </c>
+      <c r="R2" s="23">
+        <v>14</v>
+      </c>
+      <c r="S2" s="23">
+        <v>15</v>
+      </c>
+      <c r="T2" s="23">
+        <v>16</v>
+      </c>
+      <c r="U2" s="23">
+        <v>17</v>
+      </c>
+      <c r="V2" s="23">
+        <v>18</v>
+      </c>
+      <c r="W2" s="23">
+        <v>19</v>
+      </c>
+      <c r="X2" s="23">
+        <v>20</v>
+      </c>
+      <c r="Y2" s="23">
+        <v>21</v>
+      </c>
+      <c r="Z2" s="23">
+        <v>22</v>
+      </c>
+      <c r="AA2" s="23">
+        <v>23</v>
+      </c>
+      <c r="AB2" s="23">
+        <v>24</v>
+      </c>
+      <c r="AC2" s="23">
+        <v>25</v>
+      </c>
+      <c r="AD2" s="23">
+        <v>26</v>
+      </c>
+      <c r="AE2" s="23">
+        <v>27</v>
+      </c>
+      <c r="AF2" s="23">
+        <v>28</v>
+      </c>
+      <c r="AG2" s="23">
+        <v>29</v>
+      </c>
+      <c r="AH2" s="23">
+        <v>30</v>
+      </c>
+      <c r="AI2" s="23">
+        <v>31</v>
+      </c>
+      <c r="AJ2" s="23">
+        <v>32</v>
+      </c>
+      <c r="AK2" s="23">
+        <v>33</v>
+      </c>
+      <c r="AL2" s="23">
+        <v>34</v>
+      </c>
+      <c r="AM2" s="23">
+        <v>35</v>
+      </c>
+      <c r="AN2" s="23">
+        <v>36</v>
+      </c>
+      <c r="AO2" s="23">
+        <v>37</v>
+      </c>
+      <c r="AP2" s="23">
+        <v>38</v>
+      </c>
+      <c r="AQ2" s="23">
+        <v>39</v>
+      </c>
+      <c r="AR2" s="23">
+        <v>40</v>
+      </c>
+      <c r="AS2" s="23">
+        <v>41</v>
+      </c>
+      <c r="AT2" s="23">
+        <v>42</v>
+      </c>
+      <c r="AU2" s="23">
+        <v>43</v>
+      </c>
+      <c r="AV2" s="23">
+        <v>44</v>
+      </c>
+      <c r="AW2" s="23">
+        <v>45</v>
+      </c>
+      <c r="AX2" s="23">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="4:50" x14ac:dyDescent="0.25">
+      <c r="D3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="17"/>
+      <c r="Y3" s="17"/>
+      <c r="Z3" s="17"/>
+      <c r="AA3" s="17"/>
+      <c r="AB3" s="17"/>
+      <c r="AC3" s="17"/>
+      <c r="AD3" s="17"/>
+      <c r="AE3" s="18"/>
+      <c r="AF3" s="18"/>
+      <c r="AG3" s="18"/>
+      <c r="AH3" s="18"/>
+      <c r="AI3" s="18"/>
+      <c r="AJ3" s="18"/>
+      <c r="AK3" s="18"/>
+      <c r="AL3" s="18"/>
+      <c r="AM3" s="18"/>
+      <c r="AN3" s="18"/>
+      <c r="AO3" s="19"/>
+      <c r="AP3" s="19"/>
+      <c r="AQ3" s="19"/>
+      <c r="AR3" s="19"/>
+      <c r="AS3" s="19"/>
+      <c r="AT3" s="19"/>
+      <c r="AU3" s="19"/>
+      <c r="AV3" s="19"/>
+      <c r="AW3" s="19"/>
+      <c r="AX3" s="19"/>
+    </row>
+    <row r="4" spans="4:50" x14ac:dyDescent="0.25">
+      <c r="D4" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="17"/>
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="17"/>
+      <c r="AD4" s="17"/>
+      <c r="AE4" s="18"/>
+      <c r="AF4" s="18"/>
+      <c r="AG4" s="18"/>
+      <c r="AH4" s="18"/>
+      <c r="AI4" s="18"/>
+      <c r="AJ4" s="18"/>
+      <c r="AK4" s="18"/>
+      <c r="AL4" s="18"/>
+      <c r="AM4" s="18"/>
+      <c r="AN4" s="18"/>
+      <c r="AO4" s="19"/>
+      <c r="AP4" s="19"/>
+      <c r="AQ4" s="19"/>
+      <c r="AR4" s="19"/>
+      <c r="AS4" s="19"/>
+      <c r="AT4" s="19"/>
+      <c r="AU4" s="19"/>
+      <c r="AV4" s="19"/>
+      <c r="AW4" s="19"/>
+      <c r="AX4" s="19"/>
+    </row>
+    <row r="5" spans="4:50" x14ac:dyDescent="0.25">
+      <c r="D5" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="17"/>
+      <c r="AA5" s="17"/>
+      <c r="AB5" s="17"/>
+      <c r="AC5" s="17"/>
+      <c r="AD5" s="17"/>
+      <c r="AE5" s="18"/>
+      <c r="AF5" s="18"/>
+      <c r="AG5" s="18"/>
+      <c r="AH5" s="18"/>
+      <c r="AI5" s="18"/>
+      <c r="AJ5" s="18"/>
+      <c r="AK5" s="18"/>
+      <c r="AL5" s="18"/>
+      <c r="AM5" s="18"/>
+      <c r="AN5" s="18"/>
+      <c r="AO5" s="19"/>
+      <c r="AP5" s="19"/>
+      <c r="AQ5" s="19"/>
+      <c r="AR5" s="19"/>
+      <c r="AS5" s="19"/>
+      <c r="AT5" s="19"/>
+      <c r="AU5" s="19"/>
+      <c r="AV5" s="19"/>
+      <c r="AW5" s="19"/>
+      <c r="AX5" s="19"/>
+    </row>
+    <row r="6" spans="4:50" x14ac:dyDescent="0.25">
+      <c r="D6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="17"/>
+      <c r="AA6" s="17"/>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="17"/>
+      <c r="AD6" s="17"/>
+      <c r="AE6" s="18"/>
+      <c r="AF6" s="18"/>
+      <c r="AG6" s="18"/>
+      <c r="AH6" s="18"/>
+      <c r="AI6" s="18"/>
+      <c r="AJ6" s="18"/>
+      <c r="AK6" s="18"/>
+      <c r="AL6" s="18"/>
+      <c r="AM6" s="18"/>
+      <c r="AN6" s="18"/>
+      <c r="AO6" s="19"/>
+      <c r="AP6" s="19"/>
+      <c r="AQ6" s="19"/>
+      <c r="AR6" s="19"/>
+      <c r="AS6" s="19"/>
+      <c r="AT6" s="19"/>
+      <c r="AU6" s="19"/>
+      <c r="AV6" s="19"/>
+      <c r="AW6" s="19"/>
+      <c r="AX6" s="19"/>
+    </row>
+    <row r="7" spans="4:50" x14ac:dyDescent="0.25">
+      <c r="D7" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="17"/>
+      <c r="Z7" s="17"/>
+      <c r="AA7" s="17"/>
+      <c r="AB7" s="17"/>
+      <c r="AC7" s="17"/>
+      <c r="AD7" s="17"/>
+      <c r="AE7" s="18"/>
+      <c r="AF7" s="18"/>
+      <c r="AG7" s="18"/>
+      <c r="AH7" s="18"/>
+      <c r="AI7" s="18"/>
+      <c r="AJ7" s="18"/>
+      <c r="AK7" s="18"/>
+      <c r="AL7" s="18"/>
+      <c r="AM7" s="18"/>
+      <c r="AN7" s="18"/>
+      <c r="AO7" s="19"/>
+      <c r="AP7" s="19"/>
+      <c r="AQ7" s="19"/>
+      <c r="AR7" s="19"/>
+      <c r="AS7" s="19"/>
+      <c r="AT7" s="19"/>
+      <c r="AU7" s="19"/>
+      <c r="AV7" s="19"/>
+      <c r="AW7" s="19"/>
+      <c r="AX7" s="19"/>
+    </row>
+    <row r="8" spans="4:50" x14ac:dyDescent="0.25">
+      <c r="D8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="17"/>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="17"/>
+      <c r="AC8" s="17"/>
+      <c r="AD8" s="17"/>
+      <c r="AE8" s="18"/>
+      <c r="AF8" s="18"/>
+      <c r="AG8" s="18"/>
+      <c r="AH8" s="18"/>
+      <c r="AI8" s="18"/>
+      <c r="AJ8" s="18"/>
+      <c r="AK8" s="18"/>
+      <c r="AL8" s="18"/>
+      <c r="AM8" s="18"/>
+      <c r="AN8" s="18"/>
+      <c r="AO8" s="19"/>
+      <c r="AP8" s="19"/>
+      <c r="AQ8" s="19"/>
+      <c r="AR8" s="19"/>
+      <c r="AS8" s="19"/>
+      <c r="AT8" s="19"/>
+      <c r="AU8" s="19"/>
+      <c r="AV8" s="19"/>
+      <c r="AW8" s="19"/>
+      <c r="AX8" s="19"/>
+    </row>
+    <row r="9" spans="4:50" x14ac:dyDescent="0.25">
+      <c r="D9" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="17"/>
+      <c r="Y9" s="17"/>
+      <c r="Z9" s="17"/>
+      <c r="AA9" s="17"/>
+      <c r="AB9" s="17"/>
+      <c r="AC9" s="17"/>
+      <c r="AD9" s="17"/>
+      <c r="AE9" s="18"/>
+      <c r="AF9" s="18"/>
+      <c r="AG9" s="18"/>
+      <c r="AH9" s="18"/>
+      <c r="AI9" s="18"/>
+      <c r="AJ9" s="18"/>
+      <c r="AK9" s="18"/>
+      <c r="AL9" s="18"/>
+      <c r="AM9" s="18"/>
+      <c r="AN9" s="18"/>
+      <c r="AO9" s="19"/>
+      <c r="AP9" s="19"/>
+      <c r="AQ9" s="19"/>
+      <c r="AR9" s="19"/>
+      <c r="AS9" s="19"/>
+      <c r="AT9" s="19"/>
+      <c r="AU9" s="19"/>
+      <c r="AV9" s="19"/>
+      <c r="AW9" s="19"/>
+      <c r="AX9" s="19"/>
+    </row>
+    <row r="11" spans="4:50" x14ac:dyDescent="0.25">
+      <c r="E11" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="20"/>
+      <c r="X11" s="20"/>
+      <c r="Y11" s="20"/>
+      <c r="Z11" s="20"/>
+      <c r="AA11" s="20"/>
+      <c r="AB11" s="20"/>
+      <c r="AC11" s="20"/>
+      <c r="AD11" s="20"/>
+      <c r="AE11" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF11" s="21"/>
+      <c r="AG11" s="21"/>
+      <c r="AH11" s="21"/>
+      <c r="AI11" s="21"/>
+      <c r="AJ11" s="21"/>
+      <c r="AK11" s="21"/>
+      <c r="AL11" s="21"/>
+      <c r="AM11" s="21"/>
+      <c r="AN11" s="21"/>
+      <c r="AO11" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP11" s="22"/>
+      <c r="AQ11" s="22"/>
+      <c r="AR11" s="22"/>
+      <c r="AS11" s="22"/>
+      <c r="AT11" s="22"/>
+      <c r="AU11" s="22"/>
+      <c r="AV11" s="22"/>
+      <c r="AW11" s="22"/>
+      <c r="AX11" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E11:AD11"/>
+    <mergeCell ref="AE11:AN11"/>
+    <mergeCell ref="AO11:AX11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>